<commit_message>
- change DB schema and mapping - Edit amenity weight - Edit calendar view - Create draft for view customer request
</commit_message>
<xml_diff>
--- a/doc/Amenities.xlsx
+++ b/doc/Amenities.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Documents\_CAPSTONE\capstone-ors\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$24</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>item</t>
   </si>
@@ -32,12 +35,6 @@
     <t>number</t>
   </si>
   <si>
-    <t>Văn phòng mới xây</t>
-  </si>
-  <si>
-    <t>Chưa có vật dụng</t>
-  </si>
-  <si>
     <t>thang máy</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>Sảnh</t>
   </si>
   <si>
-    <t>Phòng hội nghị</t>
-  </si>
-  <si>
     <t>phòng họp trực tuyến</t>
   </si>
   <si>
@@ -95,16 +89,58 @@
     <t>Quạt trần</t>
   </si>
   <si>
-    <t>Bàn làm việc</t>
-  </si>
-  <si>
-    <t>Bàn giám đốc</t>
-  </si>
-  <si>
-    <t>Bàn họp</t>
-  </si>
-  <si>
     <t>Khu tiếp tân</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>Hội trường</t>
+  </si>
+  <si>
+    <t>Tiện nghi căn bản (0 = ko có j)</t>
+  </si>
+  <si>
+    <t>Tiện nghi họp</t>
+  </si>
+  <si>
+    <t>Điện</t>
+  </si>
+  <si>
+    <t>Vật dụng (để sửa dc)</t>
+  </si>
+  <si>
+    <t>Máy chiếu</t>
+  </si>
+  <si>
+    <t>Bảng viết</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Đèn</t>
+  </si>
+  <si>
+    <t>Máy fax</t>
+  </si>
+  <si>
+    <t>Điện thoại bàn</t>
+  </si>
+  <si>
+    <t>Máy photocopy</t>
+  </si>
+  <si>
+    <t>Máy hủy giấy</t>
+  </si>
+  <si>
+    <t>Máy in</t>
+  </si>
+  <si>
+    <t>Bàn ghế</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dịch vụ </t>
   </si>
 </sst>
 </file>
@@ -440,167 +476,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
         <v>18</v>
       </c>
-      <c r="B18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>26</v>
+      <c r="C31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>27</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C24">
+    <sortState ref="A2:C32">
+      <sortCondition ref="C1:C24"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add date to assign repair fix bugs
</commit_message>
<xml_diff>
--- a/doc/Amenities.xlsx
+++ b/doc/Amenities.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
         <v>26</v>
@@ -707,7 +707,7 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -718,7 +718,7 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -773,7 +773,7 @@
         <v>15</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>17</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>18</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -806,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="C28">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,7 +817,7 @@
         <v>23</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -828,7 +828,7 @@
         <v>24</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>25</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>27</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>